<commit_message>
#22: Improve visualization of expected values
</commit_message>
<xml_diff>
--- a/src/test/resources/integration-test-expected-values.xlsx
+++ b/src/test/resources/integration-test-expected-values.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>A</t>
   </si>
@@ -226,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -240,20 +240,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -263,37 +249,57 @@
     <xf numFmtId="2" fontId="5" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K19"/>
+  <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,38 +593,38 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="29">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="9">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="29">
         <v>2</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="12"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="31"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="25">
         <f>MEDIAN(C9:F9)</f>
         <v>1.6025</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="24">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="25">
         <f>MEDIAN(H9:K9)</f>
         <v>2.4524999999999997</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="26"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
@@ -632,109 +638,109 @@
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="27">
         <f>MEDIAN(H10:K10)</f>
         <v>2.7149999999999999</v>
       </c>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
-      <c r="K4" s="29"/>
+      <c r="K4" s="28"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="23">
         <f>MEDIAN(C11:F11)</f>
         <v>3.2949999999999999</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="30">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="23">
         <f>MEDIAN(H11:K11)</f>
         <v>3.1875</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="32"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="33"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="29">
         <v>1</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="9">
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="29">
         <v>2</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="12"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="32">
         <v>11</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10">
+      <c r="D8" s="32"/>
+      <c r="E8" s="32">
         <v>12</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="10">
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="32">
         <v>21</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10">
+      <c r="I8" s="32"/>
+      <c r="J8" s="32">
         <v>22</v>
       </c>
-      <c r="K8" s="13"/>
+      <c r="K8" s="34"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="24">
-        <f>MEDIAN(C15:D15)</f>
+      <c r="C9" s="25">
+        <f>MEDIAN(C16:D16)</f>
         <v>1.4900000000000002</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24">
-        <f>MEDIAN(E15:F15)</f>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25">
+        <f>MEDIAN(E16:F16)</f>
         <v>1.7149999999999999</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="24">
-        <f>MEDIAN(H15:I15)</f>
+      <c r="F9" s="25"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="25">
+        <f>MEDIAN(H16:I16)</f>
         <v>2.4699999999999998</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24">
-        <f>MEDIAN(J15:K15)</f>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25">
+        <f>MEDIAN(J16:K16)</f>
         <v>2.4350000000000001</v>
       </c>
       <c r="K9" s="26"/>
@@ -744,244 +750,264 @@
         <v>1</v>
       </c>
       <c r="C10" s="27">
-        <f>MEDIAN(C16:D16)</f>
+        <f>MEDIAN(C17:D17)</f>
         <v>4.1349999999999998</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="27">
-        <f>MEDIAN(E16:F16)</f>
+        <f>MEDIAN(E17:F17)</f>
         <v>3.54</v>
       </c>
       <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="27">
-        <f>MEDIAN(H16:I16)</f>
+        <f>MEDIAN(H17:I17)</f>
         <v>2.5150000000000001</v>
       </c>
       <c r="I10" s="27"/>
       <c r="J10" s="27">
-        <f>MEDIAN(J16:K16)</f>
+        <f>MEDIAN(J17:K17)</f>
         <v>2.915</v>
       </c>
-      <c r="K10" s="29"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="30">
-        <f>MEDIAN(C17:D17)</f>
+      <c r="C11" s="23">
+        <f>MEDIAN(C18:D18)</f>
         <v>4.0250000000000004</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30">
-        <f>MEDIAN(E17:F17)</f>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23">
+        <f>MEDIAN(E18:F18)</f>
         <v>2.5649999999999999</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="30">
-        <f>MEDIAN(H17:I17)</f>
+      <c r="F11" s="23"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="23">
+        <f>MEDIAN(H18:I18)</f>
         <v>2.6</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30">
-        <f>MEDIAN(J17:K17)</f>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23">
+        <f>MEDIAN(J18:K18)</f>
         <v>3.7749999999999995</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="24"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="9">
-        <v>11</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9">
-        <v>12</v>
-      </c>
-      <c r="F13" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="C13" s="29">
+        <v>1</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="9">
-        <v>21</v>
-      </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9">
-        <v>22</v>
-      </c>
-      <c r="K13" s="12"/>
+      <c r="H13" s="29">
+        <v>2</v>
+      </c>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="31"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="32">
+        <v>11</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32">
+        <v>12</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="32">
+        <v>21</v>
+      </c>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32">
+        <v>22</v>
+      </c>
+      <c r="K14" s="34"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C15" s="35">
         <v>111</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D15" s="35">
         <v>112</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E15" s="35">
         <v>121</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F15" s="35">
         <v>122</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="11">
+      <c r="G15" s="3"/>
+      <c r="H15" s="35">
         <v>211</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I15" s="35">
         <v>212</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J15" s="35">
         <v>221</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K15" s="36">
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C16" s="9">
         <v>2.4300000000000002</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D16" s="9">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E16" s="9">
         <v>1.93</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F16" s="9">
         <v>1.5</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="15">
+      <c r="G16" s="10"/>
+      <c r="H16" s="9">
         <v>3.59</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I16" s="9">
         <v>1.35</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J16" s="9">
         <v>3.08</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K16" s="11">
         <v>1.79</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="5" t="s">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C17" s="12">
         <v>3.55</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D17" s="12">
         <v>4.72</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E17" s="12">
         <v>4.3899999999999997</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F17" s="12">
         <v>2.69</v>
       </c>
-      <c r="G16" s="19"/>
-      <c r="H16" s="18">
+      <c r="G17" s="13"/>
+      <c r="H17" s="12">
         <v>3.33</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I17" s="12">
         <v>1.7</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J17" s="12">
         <v>4.0199999999999996</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K17" s="14">
         <v>1.81</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C18" s="15">
         <v>3.81</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D18" s="15">
         <v>4.24</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E18" s="15">
         <v>3.67</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F18" s="15">
         <v>1.46</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="21">
+      <c r="G18" s="16"/>
+      <c r="H18" s="15">
         <v>1.1200000000000001</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I18" s="15">
         <v>4.08</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J18" s="15">
         <v>4.2699999999999996</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K18" s="17">
         <v>3.28</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="32">
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="H7:K7"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H3:K3"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>